<commit_message>
make the examples fail more
</commit_message>
<xml_diff>
--- a/data-raw/sherlock-example-outputs/2024/061223_JPE24_E+L_E1-2_P1_SH_RH - FAIL.xlsx
+++ b/data-raw/sherlock-example-outputs/2024/061223_JPE24_E+L_E1-2_P1_SH_RH - FAIL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emanuel\projects\jpe\grunID\data-raw\sherlock-example-outputs\2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2B72DF2-B975-442B-B2D2-26E68A332217}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{705BD51C-6B93-4747-9B06-74AD46858C40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25536" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1021,7 +1021,7 @@
   <dimension ref="A2:AO204"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E92" sqref="E92"/>
+      <selection activeCell="I92" sqref="I92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -6885,7 +6885,7 @@
         <v>45936</v>
       </c>
       <c r="I91" s="13">
-        <v>2803</v>
+        <v>13000</v>
       </c>
       <c r="J91" s="13">
         <v>2973</v>
@@ -14327,6 +14327,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B141:B144"/>
+    <mergeCell ref="B145:B148"/>
+    <mergeCell ref="B149:B152"/>
+    <mergeCell ref="B153:B156"/>
+    <mergeCell ref="B157:B160"/>
     <mergeCell ref="B161:B164"/>
     <mergeCell ref="B189:B192"/>
     <mergeCell ref="B193:B196"/>
@@ -14338,11 +14343,6 @@
     <mergeCell ref="B177:B180"/>
     <mergeCell ref="B181:B184"/>
     <mergeCell ref="B185:B188"/>
-    <mergeCell ref="B141:B144"/>
-    <mergeCell ref="B145:B148"/>
-    <mergeCell ref="B149:B152"/>
-    <mergeCell ref="B153:B156"/>
-    <mergeCell ref="B157:B160"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -14355,7 +14355,7 @@
   <dimension ref="A1:Y17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -14983,26 +14983,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a5a0c31c-142b-4324-98be-1f22eeaa284f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="114905e2-0299-4464-9b5c-0bcc75829ca8" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100ED9BB87F99202C459DCB42C998E68716" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c08ee5b878ae3ef39f2021558381f3c3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a5a0c31c-142b-4324-98be-1f22eeaa284f" xmlns:ns3="114905e2-0299-4464-9b5c-0bcc75829ca8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bc11d0d83093e52fa8472e404bfcbaef" ns2:_="" ns3:_="">
     <xsd:import namespace="a5a0c31c-142b-4324-98be-1f22eeaa284f"/>
@@ -15237,26 +15217,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F1412CB-6D94-4A5C-B7A5-9FB058386B1E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a5a0c31c-142b-4324-98be-1f22eeaa284f"/>
-    <ds:schemaRef ds:uri="114905e2-0299-4464-9b5c-0bcc75829ca8"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CBC3FDB-6B65-4514-8D94-333274499CC4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a5a0c31c-142b-4324-98be-1f22eeaa284f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="114905e2-0299-4464-9b5c-0bcc75829ca8" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A3C8F84-4C33-4311-8670-B3A08FC3537F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15273,4 +15254,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CBC3FDB-6B65-4514-8D94-333274499CC4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F1412CB-6D94-4A5C-B7A5-9FB058386B1E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a5a0c31c-142b-4324-98be-1f22eeaa284f"/>
+    <ds:schemaRef ds:uri="114905e2-0299-4464-9b5c-0bcc75829ca8"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>